<commit_message>
Model, Controller, dan Sheet Rekening
</commit_message>
<xml_diff>
--- a/src/Excel/dataProject.xlsx
+++ b/src/Excel/dataProject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4185" tabRatio="835" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4185" tabRatio="835" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Buku" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="SubKategori" sheetId="5" r:id="rId5"/>
     <sheet name="Transaksi" sheetId="6" r:id="rId6"/>
     <sheet name="DetailTransaksi" sheetId="7" r:id="rId7"/>
+    <sheet name="Rekening" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="tabelcobalah">Penulis!$B$2:$C$84</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="433">
   <si>
     <t>idBuku</t>
   </si>
@@ -1290,6 +1291,39 @@
   </si>
   <si>
     <t>DT003</t>
+  </si>
+  <si>
+    <t>No Rekening</t>
+  </si>
+  <si>
+    <t>Nama Pemilik</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>05-0311-224</t>
+  </si>
+  <si>
+    <t>05-0645-714</t>
+  </si>
+  <si>
+    <t>04-7653-991</t>
+  </si>
+  <si>
+    <t>01-4563-202</t>
+  </si>
+  <si>
+    <t>Afif</t>
+  </si>
+  <si>
+    <t>Ilham</t>
+  </si>
+  <si>
+    <t>Naufal</t>
+  </si>
+  <si>
+    <t>Rizki</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1388,7 @@
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1381,6 +1415,9 @@
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1671,13 +1708,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="24.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="2" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4421,9 +4458,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="28.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5113,9 +5150,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5213,7 +5250,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5255,9 +5292,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5330,8 +5367,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5388,13 +5425,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5451,4 +5488,79 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.50972222222222197" footer="0.50972222222222197"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C2" s="10">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C3" s="10">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C4" s="10">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" s="10">
+        <v>10000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ini source code yang ketingggalan
</commit_message>
<xml_diff>
--- a/src/Excel/dataProject.xlsx
+++ b/src/Excel/dataProject.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8370" tabRatio="835"/>
+    <workbookView tabRatio="835" windowHeight="8370" windowWidth="19890" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Buku" sheetId="1" r:id="rId1"/>
-    <sheet name="Penulis" sheetId="2" r:id="rId2"/>
-    <sheet name="Penerbit" sheetId="3" r:id="rId3"/>
-    <sheet name="Kategori" sheetId="4" r:id="rId4"/>
-    <sheet name="SubKategori" sheetId="5" r:id="rId5"/>
-    <sheet name="Transaksi" sheetId="6" r:id="rId6"/>
-    <sheet name="DetailTransaksi" sheetId="7" r:id="rId7"/>
-    <sheet name="Rekening" sheetId="8" r:id="rId8"/>
+    <sheet name="Buku" r:id="rId1" sheetId="1"/>
+    <sheet name="Penulis" r:id="rId2" sheetId="2"/>
+    <sheet name="Penerbit" r:id="rId3" sheetId="3"/>
+    <sheet name="Kategori" r:id="rId4" sheetId="4"/>
+    <sheet name="SubKategori" r:id="rId5" sheetId="5"/>
+    <sheet name="Transaksi" r:id="rId6" sheetId="6"/>
+    <sheet name="DetailTransaksi" r:id="rId7" sheetId="7"/>
+    <sheet name="Rekening" r:id="rId8" sheetId="8"/>
   </sheets>
   <definedNames>
     <definedName name="tabelcobalah">Penulis!$B$2:$C$84</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="434">
   <si>
     <t>idBuku</t>
   </si>
@@ -1332,15 +1332,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1352,349 +1349,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1717,339 +1384,54 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="41" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="6" name="Comma [0]" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
-      <color rgb="00000000"/>
+      <color rgb="FF000000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2065,10 +1447,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2232,21 +1614,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2263,7 +1645,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2312,30 +1694,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:L101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I101"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="3"/>
-    <col min="2" max="2" width="24.1428571428571" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.5714285714286" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.57142857142857" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.14285714285714" style="3"/>
-    <col min="6" max="6" width="12.2857142857143" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.14285714285714" style="3"/>
+    <col min="1" max="1" style="3" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="10.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" style="3" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="12.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2389,8 +1771,8 @@
       <c r="H2" s="10">
         <v>30000</v>
       </c>
-      <c r="I2" s="3">
-        <v>100</v>
+      <c r="I2" s="3" t="n">
+        <v>96.0</v>
       </c>
       <c r="L2" s="6"/>
     </row>
@@ -2419,8 +1801,8 @@
       <c r="H3" s="10">
         <v>35000</v>
       </c>
-      <c r="I3" s="3">
-        <v>100</v>
+      <c r="I3" s="3" t="n">
+        <v>-3.0</v>
       </c>
       <c r="L3" s="6"/>
     </row>
@@ -5365,25 +4747,23 @@
       <c r="L101" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
-  <headerFooter/>
+  <pageMargins bottom="1" footer="0.50902777777777797" header="0.50902777777777797" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="3" collapsed="1"/>
-    <col min="2" max="2" width="28.4285714285714" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="28.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6059,25 +5439,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
-  <headerFooter/>
+  <pageMargins bottom="1" footer="0.50902777777777797" header="0.50902777777777797" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.1428571428571" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.4285714285714" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="3" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="21.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6161,23 +5539,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
-  <headerFooter/>
+  <pageMargins bottom="1" footer="0.50902777777777797" header="0.50902777777777797" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6205,25 +5581,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
-  <headerFooter/>
+  <pageMargins bottom="1" footer="0.50902777777777797" header="0.50902777777777797" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85714285714286" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6282,24 +5656,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
-  <headerFooter/>
+  <pageMargins bottom="1" footer="0.50902777777777797" header="0.50902777777777797" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6347,24 +5719,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins bottom="1" footer="0.50902777777777797" header="0.50902777777777797" left="0.75" right="0.75" top="1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6419,25 +5789,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
-  <headerFooter/>
+  <pageMargins bottom="1" footer="0.50902777777777797" header="0.50902777777777797" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="12.5714285714286" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6496,7 +5864,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>